<commit_message>
Completed Protecting Specific Cells in a Worksheet
</commit_message>
<xml_diff>
--- a/27 - Auditing a Worksheet/Excel103-AdvancedExercises.xlsx
+++ b/27 - Auditing a Worksheet/Excel103-AdvancedExercises.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="1565" documentId="13_ncr:1_{6BF69C48-EB2D-479A-8B64-84A9AC67A521}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{97749B83-6BCB-4216-8579-9F5339728E50}"/>
   <bookViews>
-    <workbookView xWindow="-16560" yWindow="-103" windowWidth="16663" windowHeight="8863" firstSheet="10" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-16560" yWindow="-103" windowWidth="16663" windowHeight="8863" firstSheet="11" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="IF Function" sheetId="4" r:id="rId1"/>
@@ -1968,13 +1968,13 @@
     <xf numFmtId="0" fontId="16" fillId="8" borderId="17" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="8" borderId="3" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4903,10 +4903,10 @@
       <c r="C2" s="40" t="s">
         <v>18</v>
       </c>
-      <c r="E2" s="132" t="s">
+      <c r="E2" s="130" t="s">
         <v>166</v>
       </c>
-      <c r="F2" s="132"/>
+      <c r="F2" s="130"/>
     </row>
     <row r="3" spans="2:6" ht="13">
       <c r="B3" s="25" t="s">
@@ -4915,11 +4915,11 @@
       <c r="C3" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="E3" s="130" t="str">
+      <c r="E3" s="131" t="str">
         <f>CONCATENATE(C3," ",B3)</f>
         <v>Howard Smith</v>
       </c>
-      <c r="F3" s="131"/>
+      <c r="F3" s="132"/>
     </row>
     <row r="4" spans="2:6" ht="13">
       <c r="B4" s="25" t="s">
@@ -4928,11 +4928,11 @@
       <c r="C4" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="E4" s="130" t="str">
+      <c r="E4" s="131" t="str">
         <f>CONCATENATE(C4," ",B4)</f>
         <v>Joe Gonzales</v>
       </c>
-      <c r="F4" s="131"/>
+      <c r="F4" s="132"/>
     </row>
     <row r="5" spans="2:6" ht="13">
       <c r="B5" s="25" t="s">
@@ -4941,11 +4941,11 @@
       <c r="C5" s="25" t="s">
         <v>34</v>
       </c>
-      <c r="E5" s="130" t="str">
+      <c r="E5" s="131" t="str">
         <f t="shared" ref="E5:E18" si="0">CONCATENATE(C5," ",B5)</f>
         <v>Gail Scote</v>
       </c>
-      <c r="F5" s="131"/>
+      <c r="F5" s="132"/>
     </row>
     <row r="6" spans="2:6" ht="13">
       <c r="B6" s="25" t="s">
@@ -4954,11 +4954,11 @@
       <c r="C6" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="E6" s="130" t="str">
+      <c r="E6" s="131" t="str">
         <f t="shared" si="0"/>
         <v>Sheryl Kane</v>
       </c>
-      <c r="F6" s="131"/>
+      <c r="F6" s="132"/>
     </row>
     <row r="7" spans="2:6" ht="13">
       <c r="B7" s="25" t="s">
@@ -4967,11 +4967,11 @@
       <c r="C7" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="E7" s="130" t="str">
+      <c r="E7" s="131" t="str">
         <f t="shared" si="0"/>
         <v>Kendrick Hapsbuch</v>
       </c>
-      <c r="F7" s="131"/>
+      <c r="F7" s="132"/>
     </row>
     <row r="8" spans="2:6" ht="13">
       <c r="B8" s="25" t="s">
@@ -4980,11 +4980,11 @@
       <c r="C8" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="E8" s="130" t="str">
+      <c r="E8" s="131" t="str">
         <f t="shared" si="0"/>
         <v>Mark Henders</v>
       </c>
-      <c r="F8" s="131"/>
+      <c r="F8" s="132"/>
     </row>
     <row r="9" spans="2:6" ht="13">
       <c r="B9" s="25" t="s">
@@ -4993,11 +4993,11 @@
       <c r="C9" s="25" t="s">
         <v>49</v>
       </c>
-      <c r="E9" s="130" t="str">
+      <c r="E9" s="131" t="str">
         <f t="shared" si="0"/>
         <v>Katie Atherton</v>
       </c>
-      <c r="F9" s="131"/>
+      <c r="F9" s="132"/>
     </row>
     <row r="10" spans="2:6" ht="13">
       <c r="B10" s="25" t="s">
@@ -5006,11 +5006,11 @@
       <c r="C10" s="25" t="s">
         <v>53</v>
       </c>
-      <c r="E10" s="130" t="str">
+      <c r="E10" s="131" t="str">
         <f t="shared" si="0"/>
         <v>Frank Bellwood</v>
       </c>
-      <c r="F10" s="131"/>
+      <c r="F10" s="132"/>
     </row>
     <row r="11" spans="2:6" ht="13">
       <c r="B11" s="25" t="s">
@@ -5019,11 +5019,11 @@
       <c r="C11" s="25" t="s">
         <v>57</v>
       </c>
-      <c r="E11" s="130" t="str">
+      <c r="E11" s="131" t="str">
         <f t="shared" si="0"/>
         <v>Linda Cooper</v>
       </c>
-      <c r="F11" s="131"/>
+      <c r="F11" s="132"/>
     </row>
     <row r="12" spans="2:6" ht="13">
       <c r="B12" s="25" t="s">
@@ -5032,11 +5032,11 @@
       <c r="C12" s="25" t="s">
         <v>60</v>
       </c>
-      <c r="E12" s="130" t="str">
+      <c r="E12" s="131" t="str">
         <f t="shared" si="0"/>
         <v>Brent Cronwith</v>
       </c>
-      <c r="F12" s="131"/>
+      <c r="F12" s="132"/>
     </row>
     <row r="13" spans="2:6" ht="13">
       <c r="B13" s="25" t="s">
@@ -5045,11 +5045,11 @@
       <c r="C13" s="25" t="s">
         <v>63</v>
       </c>
-      <c r="E13" s="130" t="str">
+      <c r="E13" s="131" t="str">
         <f t="shared" si="0"/>
         <v>Sandrae Simpson</v>
       </c>
-      <c r="F13" s="131"/>
+      <c r="F13" s="132"/>
     </row>
     <row r="14" spans="2:6" ht="13">
       <c r="B14" s="25" t="s">
@@ -5058,11 +5058,11 @@
       <c r="C14" s="25" t="s">
         <v>67</v>
       </c>
-      <c r="E14" s="130" t="str">
+      <c r="E14" s="131" t="str">
         <f t="shared" si="0"/>
         <v>Randy Sindole</v>
       </c>
-      <c r="F14" s="131"/>
+      <c r="F14" s="132"/>
     </row>
     <row r="15" spans="2:6" ht="13">
       <c r="B15" s="25" t="s">
@@ -5071,11 +5071,11 @@
       <c r="C15" s="25" t="s">
         <v>69</v>
       </c>
-      <c r="E15" s="130" t="str">
+      <c r="E15" s="131" t="str">
         <f t="shared" si="0"/>
         <v>Ellen Smith</v>
       </c>
-      <c r="F15" s="131"/>
+      <c r="F15" s="132"/>
     </row>
     <row r="16" spans="2:6" ht="13">
       <c r="B16" s="25" t="s">
@@ -5084,11 +5084,11 @@
       <c r="C16" s="25" t="s">
         <v>72</v>
       </c>
-      <c r="E16" s="130" t="str">
+      <c r="E16" s="131" t="str">
         <f t="shared" si="0"/>
         <v>Tuome Vuanuo</v>
       </c>
-      <c r="F16" s="131"/>
+      <c r="F16" s="132"/>
     </row>
     <row r="17" spans="2:6" ht="13">
       <c r="B17" s="25" t="s">
@@ -5097,11 +5097,11 @@
       <c r="C17" s="25" t="s">
         <v>75</v>
       </c>
-      <c r="E17" s="130" t="str">
+      <c r="E17" s="131" t="str">
         <f t="shared" si="0"/>
         <v>Tadeuz Szcznyck</v>
       </c>
-      <c r="F17" s="131"/>
+      <c r="F17" s="132"/>
     </row>
     <row r="18" spans="2:6" ht="13">
       <c r="B18" s="25" t="s">
@@ -5110,14 +5110,21 @@
       <c r="C18" s="25" t="s">
         <v>78</v>
       </c>
-      <c r="E18" s="130" t="str">
+      <c r="E18" s="131" t="str">
         <f t="shared" si="0"/>
         <v>Tammy Wu</v>
       </c>
-      <c r="F18" s="131"/>
+      <c r="F18" s="132"/>
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="E17:F17"/>
     <mergeCell ref="E2:F2"/>
     <mergeCell ref="E3:F3"/>
     <mergeCell ref="E4:F4"/>
@@ -5128,13 +5135,6 @@
     <mergeCell ref="E6:F6"/>
     <mergeCell ref="E7:F7"/>
     <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="E17:F17"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -5147,8 +5147,8 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:I14"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView showGridLines="0" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5"/>
@@ -5420,7 +5420,7 @@
   <sheetPr codeName="Sheet7"/>
   <dimension ref="A2:B2"/>
   <sheetViews>
-    <sheetView zoomScale="295" zoomScaleNormal="295" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="295" zoomScaleNormal="295" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>

</xml_diff>